<commit_message>
refactor: change folder name
</commit_message>
<xml_diff>
--- a/U2/LW1/movies.xlsx
+++ b/U2/LW1/movies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garfo/DM'22/U2/LW1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7BECC1-98A8-0044-84B6-D04B807484BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F21C9D-2D93-6343-8178-DD8D04FD8FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{438E8829-FFC3-AE4D-B306-B4E01041DB70}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18280" xr2:uid="{438E8829-FFC3-AE4D-B306-B4E01041DB70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
-  <si>
-    <t>movie_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="85">
   <si>
     <t>movie_name</t>
   </si>
@@ -46,12 +43,6 @@
     <t>movie_year</t>
   </si>
   <si>
-    <t>movie_genre</t>
-  </si>
-  <si>
-    <t>movie_duration</t>
-  </si>
-  <si>
     <t>Apocalypto</t>
   </si>
   <si>
@@ -61,9 +52,6 @@
     <t>Science-Fiction</t>
   </si>
   <si>
-    <t>Action</t>
-  </si>
-  <si>
     <t>Psycho</t>
   </si>
   <si>
@@ -100,9 +88,6 @@
     <t>American Psycho</t>
   </si>
   <si>
-    <t>Fight Club</t>
-  </si>
-  <si>
     <t>Ratatouille</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t>Her</t>
   </si>
   <si>
-    <t>Romance</t>
-  </si>
-  <si>
     <t>Interstellar</t>
   </si>
   <si>
@@ -145,9 +127,6 @@
     <t>Parasite</t>
   </si>
   <si>
-    <t>History</t>
-  </si>
-  <si>
     <t>Little Women</t>
   </si>
   <si>
@@ -175,9 +154,6 @@
     <t>La La Land</t>
   </si>
   <si>
-    <t>Music</t>
-  </si>
-  <si>
     <t>Call Me by Your Name</t>
   </si>
   <si>
@@ -233,13 +209,94 @@
   </si>
   <si>
     <t>Leto</t>
+  </si>
+  <si>
+    <t>Wild Settings</t>
+  </si>
+  <si>
+    <t>Action/Adventure/Thriller</t>
+  </si>
+  <si>
+    <t>Musical</t>
+  </si>
+  <si>
+    <t>Music Stars</t>
+  </si>
+  <si>
+    <t>Political/Historical</t>
+  </si>
+  <si>
+    <t>High Sci-fi</t>
+  </si>
+  <si>
+    <t>Low Magic</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Abuse</t>
+  </si>
+  <si>
+    <t>Animation/Comedy/Musical</t>
+  </si>
+  <si>
+    <t>Anime</t>
+  </si>
+  <si>
+    <t>Traditional</t>
+  </si>
+  <si>
+    <t>Alcoholism</t>
+  </si>
+  <si>
+    <t>High Magic</t>
+  </si>
+  <si>
+    <t>Low Sci-fi</t>
+  </si>
+  <si>
+    <t>Melodrama</t>
+  </si>
+  <si>
+    <t>Poverty</t>
+  </si>
+  <si>
+    <t>Romantic</t>
+  </si>
+  <si>
+    <t>Dance</t>
+  </si>
+  <si>
+    <t>Theatrical</t>
+  </si>
+  <si>
+    <t>Historical/ Political</t>
+  </si>
+  <si>
+    <t>Historical</t>
+  </si>
+  <si>
+    <t>level 1</t>
+  </si>
+  <si>
+    <t>level 2</t>
+  </si>
+  <si>
+    <t>level 3</t>
+  </si>
+  <si>
+    <t>movie_   duration</t>
+  </si>
+  <si>
+    <t>movie_ id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -260,6 +317,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -329,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -347,6 +410,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,892 +728,1175 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="50.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="7">
         <v>2006</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5">
+        <v>59</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="5">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="7">
         <v>2021</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="7">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="7">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="7">
         <v>1960</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7">
+        <v>59</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="7">
         <v>1982</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="7">
         <v>118</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="7">
         <v>1971</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="7">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="7">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="7">
         <v>2004</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="7">
+        <v>67</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="7">
         <v>119</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" s="7">
         <v>1994</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="7">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="7">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C9" s="7">
         <v>1991</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="7">
+        <v>59</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="7">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10" s="7">
         <v>2001</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="7">
+        <v>67</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="7">
         <v>125</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="7">
         <v>2001</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="7">
+        <v>67</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="7">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C12" s="7">
         <v>2000</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="7">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="7">
         <v>102</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" s="7">
-        <v>199</v>
+        <v>2007</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="7">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="7">
+        <v>111</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C14" s="7">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="7">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="7">
+        <v>162</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C15" s="7">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="7">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="7">
+        <v>148</v>
+      </c>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C16" s="7">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="7">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C17" s="7">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="7">
+        <v>142</v>
+      </c>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="7">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="7">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C19" s="7">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="7">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="7">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C20" s="7">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="7">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="7">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C21" s="7">
         <v>2017</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="7">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C22" s="7">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="7">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="7">
+        <v>101</v>
+      </c>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C23" s="7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="7">
-        <v>101</v>
-      </c>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="7">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C24" s="7">
-        <v>2019</v>
+        <v>1994</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="7">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="7">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>59</v>
+      <c r="B25" s="8">
+        <v>1917</v>
       </c>
       <c r="C25" s="7">
-        <v>1994</v>
+        <v>2019</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="7">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="7">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="8">
-        <v>1917</v>
+      <c r="B26" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="C26" s="7">
         <v>2019</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="7">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C27" s="7">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="7">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C28" s="7">
-        <v>2021</v>
+        <v>1999</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="7">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="7">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C29" s="7">
-        <v>1999</v>
+        <v>2001</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="7">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C30" s="7">
         <v>2001</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="7">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C31" s="7">
-        <v>2001</v>
+        <v>2015</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="7">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="7">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C32" s="7">
         <v>2015</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="7">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="7">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C33" s="7">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="7">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="7">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C34" s="7">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="7">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C35" s="7">
-        <v>2017</v>
+        <v>2008</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="7">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C36" s="7">
-        <v>2008</v>
+        <v>2021</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="7">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C37" s="7">
-        <v>2021</v>
+        <v>2011</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="7">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" s="7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C38" s="7">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="7">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C39" s="7">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" s="7">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C40" s="7">
-        <v>2021</v>
+        <v>2009</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C41" s="7">
-        <v>2009</v>
+        <v>2021</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="7">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C42" s="7">
-        <v>2021</v>
+        <v>1986</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="7">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" s="7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C43" s="7">
-        <v>1986</v>
+        <v>1982</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="7">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G43" s="7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C44" s="7">
-        <v>1982</v>
+        <v>2000</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E44" s="7">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C45" s="7">
-        <v>2000</v>
+        <v>1994</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E45" s="7">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C46" s="7">
-        <v>1994</v>
+        <v>2012</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="7">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" s="7">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C47" s="7">
-        <v>2012</v>
+        <v>1977</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="7">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47" s="7">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C48" s="7">
-        <v>1977</v>
+        <v>1979</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E48" s="7">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C49" s="7">
-        <v>1979</v>
+        <v>2020</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="7">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G49" s="7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C50" s="7">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="7">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
-        <v>50</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="7">
-        <v>2018</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E51" s="7">
+        <v>67</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="7">
         <v>126</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="35" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>